<commit_message>
Confiabilidad WH, Nuevas ST
</commit_message>
<xml_diff>
--- a/BaseDeDatos/Holt Exponential Trend_metricas.xlsx
+++ b/BaseDeDatos/Holt Exponential Trend_metricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,31 @@
           <t>Entregas Minion Mega</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tarjetas credito vigentes otros</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Numero de operaciones realizadas con tarjetas de crédito</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Tarjetas vigentes</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Tarjetas vigentes VISA</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Tarjetas vigentes MASTERCARD</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -585,6 +610,21 @@
       <c r="S2" t="n">
         <v>0.4859937556822533</v>
       </c>
+      <c r="T2" t="n">
+        <v>0.1515117755174033</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.04893548824463104</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.03035588416534699</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.04510072663549621</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.02048521563172385</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -646,6 +686,21 @@
       <c r="S3" t="n">
         <v>221.4618644675527</v>
       </c>
+      <c r="T3" t="n">
+        <v>67254.58748056635</v>
+      </c>
+      <c r="U3" t="n">
+        <v>402297.5488382598</v>
+      </c>
+      <c r="V3" t="n">
+        <v>12294202.13725019</v>
+      </c>
+      <c r="W3" t="n">
+        <v>2096838.884939871</v>
+      </c>
+      <c r="X3" t="n">
+        <v>594844.9597643962</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -706,6 +761,97 @@
       </c>
       <c r="S4" t="n">
         <v>0.641777867183575</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.3678116291786256</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.08291884173554066</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.05813484878731042</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.08886124252627792</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.04251739920413474</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Confiabilidad 80%</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="V5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>